<commit_message>
arquivo de documentação atualizado com relatório até a coluna U
</commit_message>
<xml_diff>
--- a/Documentação_CovêniosSaída.xlsx
+++ b/Documentação_CovêniosSaída.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2cb3d3d3ab363be3/git/dadosAbertosSEGOVMG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_A00C3EBA7D9A6D2C82DA887ABCFB0D7B6A61C7FA" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{25F3FD0D-0DE4-49F5-886B-ADDD059E2329}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_A00C3EBA7D9A6D2C82DA887ABCFB0D7B6A61C7FA" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{092C1496-E850-4E8B-9D2D-CDC24D82B0E1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="71">
   <si>
     <t>Nome</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Formato dos dados</t>
   </si>
   <si>
-    <t>Relatórios contendo o status e a execução das emendas parlamentares - Emendas 2020</t>
-  </si>
-  <si>
     <t>Execução das emendas parlamentares - Emendas 2020</t>
   </si>
   <si>
@@ -87,6 +84,156 @@
   </si>
   <si>
     <t>Nome do Relatório</t>
+  </si>
+  <si>
+    <t>valores_indicados_emendas_impos</t>
+  </si>
+  <si>
+    <t>responsavel</t>
+  </si>
+  <si>
+    <t>uo</t>
+  </si>
+  <si>
+    <t>orgao</t>
+  </si>
+  <si>
+    <t>n_sigcon</t>
+  </si>
+  <si>
+    <t>tipo_indicacao</t>
+  </si>
+  <si>
+    <t>ano_inciso</t>
+  </si>
+  <si>
+    <t>impositividade</t>
+  </si>
+  <si>
+    <t>municipio</t>
+  </si>
+  <si>
+    <t>razao_social</t>
+  </si>
+  <si>
+    <t>cnpj</t>
+  </si>
+  <si>
+    <t>codesc</t>
+  </si>
+  <si>
+    <t>acao</t>
+  </si>
+  <si>
+    <t>grupo_despesa</t>
+  </si>
+  <si>
+    <t>genero</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>especificacao</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>tipo_aplicacao</t>
+  </si>
+  <si>
+    <t>vl_indicado</t>
+  </si>
+  <si>
+    <t>data_indicacao_sigcon</t>
+  </si>
+  <si>
+    <t>vl_informado</t>
+  </si>
+  <si>
+    <t>Responsável pela emenda</t>
+  </si>
+  <si>
+    <t>Unidade Organizacional</t>
+  </si>
+  <si>
+    <t>Órgão</t>
+  </si>
+  <si>
+    <t>Tipo de Indicação</t>
+  </si>
+  <si>
+    <t>pode ser deputado etc</t>
+  </si>
+  <si>
+    <t>Ano do Inciso</t>
+  </si>
+  <si>
+    <t>Impositividade</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Município</t>
+  </si>
+  <si>
+    <t>Razão Social</t>
+  </si>
+  <si>
+    <t>Razão social do beneficiário</t>
+  </si>
+  <si>
+    <t>CNPJ</t>
+  </si>
+  <si>
+    <t>CNPJ do beneficiário</t>
+  </si>
+  <si>
+    <t>Ação</t>
+  </si>
+  <si>
+    <t>Ação da LOA 2020</t>
+  </si>
+  <si>
+    <t>Grupo de Despesa</t>
+  </si>
+  <si>
+    <t>Grupo de despesa LOA 2020</t>
+  </si>
+  <si>
+    <t>Número de Referência SIGCON</t>
+  </si>
+  <si>
+    <t>Código Escola</t>
+  </si>
+  <si>
+    <t>Código das escolas, intitutos e centros educacionais</t>
+  </si>
+  <si>
+    <t>Gênero</t>
+  </si>
+  <si>
+    <t>Gênero da despesa</t>
+  </si>
+  <si>
+    <t>Especificação</t>
+  </si>
+  <si>
+    <t>Tipo de Aplicação</t>
+  </si>
+  <si>
+    <t>Valor Indicado</t>
+  </si>
+  <si>
+    <t>Data da Indicação no SIGCON</t>
+  </si>
+  <si>
+    <t>Valor Informado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relatórios contendo o status e a execução das emendas parlamentares - Emendas 2020. </t>
   </si>
 </sst>
 </file>
@@ -164,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -173,6 +320,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -395,7 +544,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -408,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -416,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -424,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -432,7 +581,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -440,7 +589,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -448,7 +597,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -456,10 +605,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -472,7 +621,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -493,7 +642,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -503,7 +652,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
@@ -522,75 +671,285 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E25" s="3"/>
     </row>
   </sheetData>

</xml_diff>